<commit_message>
Fixed flow_step_1_output and produced output_flow
</commit_message>
<xml_diff>
--- a/flow_data_step1_output.xlsx
+++ b/flow_data_step1_output.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Desktop\GM2 Technology for the poorest\final presentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AE929B-D543-4336-BC83-D2D0551EAF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="21825" windowHeight="14025"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -107,37 +101,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ingredient_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>weight in grams</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Rice</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Salt</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INGREDIENT_NAME</t>
+  </si>
+  <si>
+    <t>WEIGHT_IN_G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -167,7 +159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -437,23 +429,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="21" max="21" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -512,13 +508,16 @@
         <v>25</v>
       </c>
       <c r="U1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="V1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22">
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="G2" t="s">
         <v>17</v>
       </c>
@@ -547,7 +546,10 @@
         <v>173.6</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22">
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
@@ -576,13 +578,16 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V3">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22">
+      <c r="C4">
+        <v>1</v>
+      </c>
       <c r="G4" t="s">
         <v>19</v>
       </c>
@@ -611,13 +616,16 @@
         <v>2</v>
       </c>
       <c r="U4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="V4">
         <v>1.23</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22">
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="G5" t="s">
         <v>21</v>
       </c>

</xml_diff>